<commit_message>
Balancing testing in Code
</commit_message>
<xml_diff>
--- a/VW GTE E-Golf Can/VW GTE Canbus Ids.xlsx
+++ b/VW GTE E-Golf Can/VW GTE Canbus Ids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomde\Documents\Electric Drives\OEM\VW\GTE Pack Can captures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DA84EE1-80F2-461B-B4D2-D720EC8487AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364AF8F2-90AA-4948-8CD2-B1C810DE0583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E944DFBD-9142-4058-966A-3AEDE6B3BAAE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="177">
   <si>
     <t>ID</t>
   </si>
@@ -557,6 +557,15 @@
   </si>
   <si>
     <t>0x00</t>
+  </si>
+  <si>
+    <t>And Balancing state</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -951,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFBAA877-7B05-4C47-AACE-4F436ACC28E0}">
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:A67"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1483,7 +1492,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>24</v>
       </c>
@@ -1493,162 +1502,171 @@
       <c r="C65" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E65" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B66" t="s">
-        <v>119</v>
-      </c>
       <c r="C66" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H66" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B67" t="s">
-        <v>120</v>
-      </c>
       <c r="C67" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H67" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B68" t="s">
-        <v>121</v>
-      </c>
       <c r="C68" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H68" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B69" t="s">
-        <v>122</v>
-      </c>
       <c r="C69" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H69" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B70" t="s">
-        <v>123</v>
-      </c>
       <c r="C70" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H70" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B71" t="s">
-        <v>124</v>
-      </c>
       <c r="C71" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H71" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B72" t="s">
-        <v>125</v>
-      </c>
       <c r="C72" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H72" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B73" t="s">
-        <v>126</v>
-      </c>
       <c r="C73" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H73" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B74" t="s">
-        <v>127</v>
-      </c>
       <c r="C74" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H74" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B75" t="s">
-        <v>128</v>
-      </c>
       <c r="C75" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H75" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B76" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C76" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H76" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B77" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C77" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H77" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B78" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C78" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B79" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C79" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>69</v>
       </c>
@@ -1674,9 +1692,6 @@
       <c r="A82" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B82" t="s">
-        <v>133</v>
-      </c>
       <c r="C82" t="s">
         <v>137</v>
       </c>
@@ -1684,9 +1699,6 @@
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B83" t="s">
-        <v>134</v>
       </c>
       <c r="C83" t="s">
         <v>137</v>
@@ -1763,10 +1775,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB91E74-3689-4080-B77F-D50F0346E3DF}">
-  <dimension ref="A2:I14"/>
+  <dimension ref="A2:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2040,6 +2052,132 @@
         <v>172</v>
       </c>
     </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1</v>
+      </c>
+      <c r="D17" s="6">
+        <v>2</v>
+      </c>
+      <c r="L17" s="6">
+        <v>3</v>
+      </c>
+      <c r="T17" s="6">
+        <v>4</v>
+      </c>
+      <c r="U17" s="6">
+        <v>5</v>
+      </c>
+      <c r="V17" s="6">
+        <v>6</v>
+      </c>
+      <c r="W17" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="D18" s="3">
+        <v>7</v>
+      </c>
+      <c r="E18" s="3">
+        <v>6</v>
+      </c>
+      <c r="F18" s="3">
+        <v>5</v>
+      </c>
+      <c r="G18" s="3">
+        <v>4</v>
+      </c>
+      <c r="H18" s="3">
+        <v>3</v>
+      </c>
+      <c r="I18" s="3">
+        <v>2</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3">
+        <v>7</v>
+      </c>
+      <c r="M18" s="3">
+        <v>6</v>
+      </c>
+      <c r="N18" s="3">
+        <v>5</v>
+      </c>
+      <c r="O18" s="3">
+        <v>4</v>
+      </c>
+      <c r="P18" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>2</v>
+      </c>
+      <c r="R18" s="3">
+        <v>1</v>
+      </c>
+      <c r="S18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D19" t="s">
+        <v>163</v>
+      </c>
+      <c r="E19" t="s">
+        <v>162</v>
+      </c>
+      <c r="F19" t="s">
+        <v>161</v>
+      </c>
+      <c r="G19" t="s">
+        <v>160</v>
+      </c>
+      <c r="H19" t="s">
+        <v>159</v>
+      </c>
+      <c r="I19" t="s">
+        <v>158</v>
+      </c>
+      <c r="J19" t="s">
+        <v>157</v>
+      </c>
+      <c r="K19" t="s">
+        <v>156</v>
+      </c>
+      <c r="P19" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>166</v>
+      </c>
+      <c r="R19" t="s">
+        <v>165</v>
+      </c>
+      <c r="S19" t="s">
+        <v>164</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>